<commit_message>
DDT Testing For CURA Login
</commit_message>
<xml_diff>
--- a/Data Files/Data_File_CURA/test_data_Cura_Login_001.xlsx
+++ b/Data Files/Data_File_CURA/test_data_Cura_Login_001.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mansurshaik\git\SI-GuidedProject-706021-1706005466\Data Files\Data_File_CURA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{BB00EA4A-8A00-462D-B8E7-240ED32C5258}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{028CF2E3-FDFA-4E9B-83CB-D560A7EAAF03}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{C699A6CA-7BCE-4B60-A167-E6CF67FD1880}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="5">
   <si>
     <t>Username</t>
   </si>
@@ -46,6 +46,9 @@
   </si>
   <si>
     <t>ThisIsNotAPassword</t>
+  </si>
+  <si>
+    <t>thisisnotapassword</t>
   </si>
 </sst>
 </file>
@@ -397,10 +400,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1FDA192A-D4DF-4323-BEE2-828B335831C9}">
-  <dimension ref="A1:B2"/>
+  <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -425,6 +428,14 @@
         <v>3</v>
       </c>
     </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>4</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>